<commit_message>
bug fixed add tags
</commit_message>
<xml_diff>
--- a/Dttfeedback.xlsx
+++ b/Dttfeedback.xlsx
@@ -140,7 +140,7 @@
     <t>All works fine. It would have been better if tags could be linked to the facility in the create call as well. But there is a functioning API call present to add tags to a facility.</t>
   </si>
   <si>
-    <t>Done. Transactions were needed.</t>
+    <t>Done. Transactions were needed. Add transactions in add tags as well</t>
   </si>
   <si>
     <t>I want to be able to Read facilities and their tags.</t>
@@ -483,7 +483,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -683,13 +683,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -788,10 +782,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1046,13 +1040,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1365,10 +1353,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>